<commit_message>
Erweiterung um 2D Pooling
</commit_message>
<xml_diff>
--- a/LaTeX/Quellen/BerechnungMinipool.xlsx
+++ b/LaTeX/Quellen/BerechnungMinipool.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="576" yWindow="84" windowWidth="29604" windowHeight="13776" activeTab="1"/>
+    <workbookView xWindow="576" yWindow="84" windowWidth="29604" windowHeight="13776" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Diagramm2" sheetId="5" r:id="rId1"/>
     <sheet name="Tabelle1" sheetId="1" r:id="rId2"/>
+    <sheet name="Schaubild2D" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="36">
   <si>
     <t>Prävalenz</t>
   </si>
@@ -52,6 +53,78 @@
   <si>
     <t>Optimum</t>
   </si>
+  <si>
+    <t>Pool-A1</t>
+  </si>
+  <si>
+    <t>Pool-A2</t>
+  </si>
+  <si>
+    <t>Pool-A3</t>
+  </si>
+  <si>
+    <t>Pool-A4</t>
+  </si>
+  <si>
+    <t>Pool-B1</t>
+  </si>
+  <si>
+    <t>Pool-B2</t>
+  </si>
+  <si>
+    <t>Pool-B3</t>
+  </si>
+  <si>
+    <t>Pool-B4</t>
+  </si>
+  <si>
+    <t>Probe11</t>
+  </si>
+  <si>
+    <t>Probe12</t>
+  </si>
+  <si>
+    <t>Probe13</t>
+  </si>
+  <si>
+    <t>Probe14</t>
+  </si>
+  <si>
+    <t>Probe21</t>
+  </si>
+  <si>
+    <t>Probe31</t>
+  </si>
+  <si>
+    <t>Probe41</t>
+  </si>
+  <si>
+    <t>Probe22</t>
+  </si>
+  <si>
+    <t>Probe23</t>
+  </si>
+  <si>
+    <t>Probe24</t>
+  </si>
+  <si>
+    <t>Probe32</t>
+  </si>
+  <si>
+    <t>Probe33</t>
+  </si>
+  <si>
+    <t>Probe34</t>
+  </si>
+  <si>
+    <t>Probe42</t>
+  </si>
+  <si>
+    <t>Probe43</t>
+  </si>
+  <si>
+    <t>Probe44</t>
+  </si>
 </sst>
 </file>
 
@@ -73,12 +146,48 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -94,10 +203,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
@@ -2940,25 +3055,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="140587392"/>
-        <c:axId val="140588928"/>
+        <c:axId val="144403840"/>
+        <c:axId val="144426112"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="140587392"/>
+        <c:axId val="144403840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="140588928"/>
+        <c:crossAx val="144426112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="140588928"/>
+        <c:axId val="144426112"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -2967,14 +3082,13 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="140587392"/>
+        <c:crossAx val="144403840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -3306,7 +3420,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:L103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -8282,4 +8396,178 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:N5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="5" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="7.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="21" customHeight="1">
+      <c r="B1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="21" customHeight="1">
+      <c r="A2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="21" customHeight="1">
+      <c r="A3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="21" customHeight="1">
+      <c r="A4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="21" customHeight="1">
+      <c r="A5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Zwischenspeichern. Pooling eindimensional analysiert.
</commit_message>
<xml_diff>
--- a/LaTeX/Quellen/BerechnungMinipool.xlsx
+++ b/LaTeX/Quellen/BerechnungMinipool.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="576" yWindow="84" windowWidth="29604" windowHeight="13776" activeTab="2"/>
+    <workbookView xWindow="576" yWindow="84" windowWidth="29604" windowHeight="13776" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Diagramm2" sheetId="5" r:id="rId1"/>
     <sheet name="Tabelle1" sheetId="1" r:id="rId2"/>
     <sheet name="Schaubild2D" sheetId="6" r:id="rId3"/>
+    <sheet name="Praevalenz" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="44">
   <si>
     <t>Prävalenz</t>
   </si>
@@ -125,11 +126,39 @@
   <si>
     <t>Probe44</t>
   </si>
+  <si>
+    <t>Schaubild Poolgröße 3 / Einzelnachtestung</t>
+  </si>
+  <si>
+    <t>Prävalenz %</t>
+  </si>
+  <si>
+    <t>Erwartung</t>
+  </si>
+  <si>
+    <t>Schaublid Prävalenz 20% / Einzelnachtestung</t>
+  </si>
+  <si>
+    <t>AlleNegativ</t>
+  </si>
+  <si>
+    <t>Gruppengröße</t>
+  </si>
+  <si>
+    <t>Prävalenz:</t>
+  </si>
+  <si>
+    <t>=Gruppengröße/(((1-PAlleNegativ)*(Gruppengröße+1))+((PAlleNegativ)*1))</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt numFmtId="171" formatCode="0.0"/>
+    <numFmt numFmtId="174" formatCode="0.000%"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -203,7 +232,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -213,6 +242,11 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
@@ -3055,25 +3089,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="144403840"/>
-        <c:axId val="144426112"/>
+        <c:axId val="186920960"/>
+        <c:axId val="186922496"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="144403840"/>
+        <c:axId val="186920960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="144426112"/>
+        <c:crossAx val="186922496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="144426112"/>
+        <c:axId val="186922496"/>
         <c:scaling>
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
@@ -3082,7 +3116,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="144403840"/>
+        <c:crossAx val="186920960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3092,6 +3126,1474 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="de-DE"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>1 Prozent</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Praevalenz!$H$6:$H$35</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>0.99965012245713991</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9972044031506684</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.9905829604077674</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.9777363681547704</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.956659577611835</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.9254051916986379</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.8820959121814251</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.8249359996168053</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.7522216095049998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.6623498939269652</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10.55382678542073</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11.42527340805149</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12.275431088671708</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13.103164968436216</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>13.907466240008169</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>14.687453058957837</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>15.442370198134626</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>16.171587530946827</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>16.874597443307803</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>17.551011284433905</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>18.200554973756475</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>18.823063885094708</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>19.418477130165666</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>19.986831361791577</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>20.52825421314931</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>21.04295748347344</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>21.531230173159223</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>21.993431462586511</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>22.429983719572881</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>22.841365610480814</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>3 Prozent</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Praevalenz!$I$6:$I$35</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>0.970873786407767</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.7885888034340904</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.3772148709053464</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.7419256527407638</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.9302657613352339</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.996751565615837</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.9861951357431753</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.9303459072686611</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.849976774110984</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.7580434170538628</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.6623523224490895</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.5674536023198735</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.4758849624331538</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.3889594108880869</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.3072549363008505</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.230916119506519</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.1598389434139067</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.0937835246254726</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.0324424385364273</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.9754816763244711</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.9225647260267946</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.8733662553382437</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.8275794091858333</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.7849192165418508</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.7451236606298686</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.7079533813867083</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.6731906129329981</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.6406377288546339</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.6101156232603391</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.5814620642585975</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>10 Prozent</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Praevalenz!$J$6:$J$35</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>0.90909090909090906</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.4492753623188408</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.6547159404302263</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.683785149014986</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.6406621712523177</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.5742436939733233</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.5047544759835492</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.4398168299584535</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.3818059395088669</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.330988026129716</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.2868381635880028</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.2485894110255731</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.2154559900808217</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.1867173383541654</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.1617430559259629</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.139993503780204</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.121011244171761</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.1044098951442851</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.0898631308179154</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.0770948457344149</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.0658707500104958</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.0559913485486214</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.0472861426432427</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.0396088653228692</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.032833571396762</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.0268514258964598</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.0215680599444594</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.016901386707435</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.0127797905005336</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.0091406190692729</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="80263040"/>
+        <c:axId val="80273792"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="80263040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="80273792"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="80273792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="80263040"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="de-DE"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>4 Testpersonen</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Praevalenz!$A$6:$A$55</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>2.9999999999999997E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.5399999999999993E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.177199999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.929095999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.8163332799999968E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.863273270399996E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.0986624590719946E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.5564217017049535E-4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.1276577608011844E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.3306361577453975E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.570150666139569E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.8527777860446915E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.186277787532736E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.5798077892886283E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.0441731913605813E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.5921243658054857E-3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.2387067516504728E-3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.0016739669475575E-3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5.9019752809981174E-3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6.9643308315777783E-3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8.2179103812617775E-3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9.6971342498888974E-3</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.1442618414868898E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.3502289729545298E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.5932701880863452E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.8800588219418872E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.2184694098914267E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.6177939036718834E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>3.0889968063328221E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3.6450162314727301E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4.3011191531378209E-2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>5.0753206007026284E-2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>5.9888783088291014E-2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>7.0668764044183388E-2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>8.3389141572136394E-2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>9.8399187055120935E-2</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.11611104072504269</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.13701102805555038</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.16167301310554943</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.19077415546454832</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.225113503448167</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.26563393406883706</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.31344804220122774</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.36986868979744869</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.43644505396098943</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.51500516367396754</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.60770609313528168</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.71709318989963233</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.84616996408156608</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.99848055761624788</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Praevalenz!$B$5:$B$55</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="51"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.9809002757016101</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.9774834932868135</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.9734599363095171</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.9687235829101333</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.963150557710807</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.9565963856503998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.948892925336458</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.9398449864966492</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.9292266577683952</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.9167774026686337</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.9021980261047458</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.8851466745588614</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.865235113528616</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.8420256288902928</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.8150290260707793</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.7837043507873505</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.7474611209185928</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.7056650258807569</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.6576481910789269</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.6027251789257986</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.5402158460736493</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.4694759255641956</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.3899356733824164</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.3011460455667256</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3.2028306332590479</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.0949400425866331</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.9777037523799663</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.8516730474155874</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.7177478564494333</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2.5771806930089132</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2.43155273537303</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2.2827204022120346</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2.1327351461969037</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1.9837437345255258</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.8378799255467377</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1.6971602220179456</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1.5633957936832548</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.4381298795270481</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.3226057447380477</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1.2177655865390256</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1.1242765149213416</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1.0425762051634602</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.97292752071046018</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.91546670689481624</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.87022057778013118</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.83705014589174243</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.81545018461294405</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.80412083198513451</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.80035854125704298</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.80000000000341132</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>8 Testpersonen</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Praevalenz!$A$6:$A$55</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>2.9999999999999997E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.5399999999999993E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.177199999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.929095999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.8163332799999968E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.863273270399996E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.0986624590719946E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.5564217017049535E-4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.1276577608011844E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.3306361577453975E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.570150666139569E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.8527777860446915E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.186277787532736E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.5798077892886283E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.0441731913605813E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.5921243658054857E-3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.2387067516504728E-3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.0016739669475575E-3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5.9019752809981174E-3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6.9643308315777783E-3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8.2179103812617775E-3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9.6971342498888974E-3</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.1442618414868898E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.3502289729545298E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.5932701880863452E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.8800588219418872E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.2184694098914267E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.6177939036718834E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>3.0889968063328221E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3.6450162314727301E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4.3011191531378209E-2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>5.0753206007026284E-2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>5.9888783088291014E-2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>7.0668764044183388E-2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>8.3389141572136394E-2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>9.8399187055120935E-2</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.11611104072504269</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.13701102805555038</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.16167301310554943</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.19077415546454832</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.225113503448167</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.26563393406883706</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.31344804220122774</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.36986868979744869</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.43644505396098943</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.51500516367396754</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.60770609313528168</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.71709318989963233</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.84616996408156608</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.99848055761624788</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Praevalenz!$C$5:$C$55</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="51"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.8494487342770478</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.8229819624887194</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.7919925494657267</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.7557569056202444</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.713454108373436</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.6641597427296579</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.6068421901071872</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.5403627063897423</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.4634809746527742</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.3748681568595016</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.273129742158126</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.1568406053677123</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7.0245945212012506</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.875069772481714</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6.7071112818789134</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.5198277611903572</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6.312699689768686</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6.0856906746918371</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5.8393513481504895</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5.5749021554952449</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5.2942801303429929</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5.0001359873887257</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4.6957721856226193</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4.3850199000356715</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4.0720620214518304</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.7612184755962383</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3.4567170594777799</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>3.1624757750948556</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.8819205158596</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2.6178555292347867</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2.3723950860143317</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2.1469554734197529</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.9422987743082019</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1.7586150729858065</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.5956279474108959</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1.4527087854582896</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1.3289875738055872</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.2234502253828157</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.1350142504724208</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1.0625749695482856</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1.0050134524714667</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.96115626427768563</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.92968026621566635</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.90897273147402669</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.89700093666640679</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.8913142434806508</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.88933229741909325</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.88892131224835735</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.88888913664490443</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.88888888888888884</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>16 Testpersonen</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Praevalenz!$A$6:$A$55</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>2.9999999999999997E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.5399999999999993E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.177199999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.929095999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.8163332799999968E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.863273270399996E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.0986624590719946E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.5564217017049535E-4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.1276577608011844E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.3306361577453975E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.570150666139569E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.8527777860446915E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.186277787532736E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.5798077892886283E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.0441731913605813E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.5921243658054857E-3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.2387067516504728E-3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.0016739669475575E-3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5.9019752809981174E-3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6.9643308315777783E-3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8.2179103812617775E-3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9.6971342498888974E-3</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.1442618414868898E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.3502289729545298E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.5932701880863452E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.8800588219418872E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.2184694098914267E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.6177939036718834E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>3.0889968063328221E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3.6450162314727301E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4.3011191531378209E-2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>5.0753206007026284E-2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>5.9888783088291014E-2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>7.0668764044183388E-2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>8.3389141572136394E-2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>9.8399187055120935E-2</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.11611104072504269</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.13701102805555038</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.16167301310554943</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.19077415546454832</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.225113503448167</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.26563393406883706</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.31344804220122774</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.36986868979744869</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.43644505396098943</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.51500516367396754</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.60770609313528168</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.71709318989963233</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.84616996408156608</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.99848055761624788</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Praevalenz!$D$5:$D$55</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="51"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14.86122253671096</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14.673732443802216</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14.458676834838638</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14.213132817023563</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13.934243390154863</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13.619359411394994</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13.266215021163546</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12.873132291911777</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12.439245047431976</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11.964724962144626</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11.450986226595836</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10.900839884891164</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>10.318567405113988</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9.709886973641277</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9.0817963477596741</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8.4422921739859582</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>7.7999848490006594</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>7.1636460832409314</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6.5417387565266809</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5.9419820342839147</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5.3709980882990429</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4.8340719971445516</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4.3350374435634222</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.8762822836677779</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3.4588536976106439</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.0826344305851845</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.7465596733245166</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.4488470791280683</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.1872182925771675</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.9590972386210093</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.761776814105108</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1.5925506504704781</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.4488099069238174</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1.3281066007377373</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.2281850088232034</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1.1469816182050332</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1.0825927929450734</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.0332094230692521</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.99702234613752172</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.97211536434600643</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.95638592807687473</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.94755731504053164</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.94333975568214079</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.94172410622491065</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.94126816960635495</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.94118477176743243</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.94117674928200123</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.94117647207978083</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.94117647058832243</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.94117647058823528</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="64968192"/>
+        <c:axId val="65208320"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="64968192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200"/>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="65208320"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:tickLblSkip val="8"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="65208320"/>
+        <c:scaling>
+          <c:logBase val="2"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200"/>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="64968192"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.7705673758865248"/>
+          <c:y val="0.39894619654024727"/>
+          <c:w val="0.21879432624113476"/>
+          <c:h val="0.21680461238641466"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200"/>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
@@ -3130,6 +4632,71 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>213360</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>594360</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Diagramm 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>480060</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>510540</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Diagramm 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -8402,7 +9969,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
@@ -8570,4 +10137,2132 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J65"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="G4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4" s="13">
+        <v>3.5E-4</v>
+      </c>
+      <c r="I4" s="12">
+        <v>0.03</v>
+      </c>
+      <c r="J4" s="12">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="B6" s="11">
+        <f>B$5/(((1-POWER((1-$A6),B$5))*(B$5+1))+(POWER((1-$A6),B$5)*1))</f>
+        <v>3.9809002757016101</v>
+      </c>
+      <c r="C6" s="11">
+        <f t="shared" ref="C6:D21" si="0">C$5/(((1-POWER((1-$A6),C$5))*(C$5+1))+(POWER((1-$A6),C$5)*1))</f>
+        <v>7.8494487342770478</v>
+      </c>
+      <c r="D6" s="11">
+        <f t="shared" si="0"/>
+        <v>14.86122253671096</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6" s="10">
+        <f>POWER((1-$H$4),F6)</f>
+        <v>0.99965000000000004</v>
+      </c>
+      <c r="H6" s="10">
+        <f>$F6/(((1-POWER((1-H$4),$F6))*($F6+1))+POWER((1-H$4),$F6))</f>
+        <v>0.99965012245713991</v>
+      </c>
+      <c r="I6" s="10">
+        <f t="shared" ref="I6:J21" si="1">$F6/(((1-POWER((1-I$4),$F6))*($F6+1))+POWER((1-I$4),$F6))</f>
+        <v>0.970873786407767</v>
+      </c>
+      <c r="J6" s="10">
+        <f t="shared" si="1"/>
+        <v>0.90909090909090906</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="1">
+        <f>A6*1.18</f>
+        <v>3.5399999999999993E-4</v>
+      </c>
+      <c r="B7" s="11">
+        <f t="shared" ref="B7:D38" si="2">B$5/(((1-POWER((1-$A7),B$5))*(B$5+1))+(POWER((1-$A7),B$5)*1))</f>
+        <v>3.9774834932868135</v>
+      </c>
+      <c r="C7" s="11">
+        <f t="shared" si="0"/>
+        <v>7.8229819624887194</v>
+      </c>
+      <c r="D7" s="11">
+        <f t="shared" si="0"/>
+        <v>14.673732443802216</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7" s="10">
+        <f>POWER((1-$H$4),F7)</f>
+        <v>0.99930012250000011</v>
+      </c>
+      <c r="H7" s="10">
+        <f t="shared" ref="H7:J36" si="3">$F7/(((1-POWER((1-H$4),$F7))*($F7+1))+POWER((1-H$4),$F7))</f>
+        <v>1.9972044031506684</v>
+      </c>
+      <c r="I7" s="10">
+        <f t="shared" si="1"/>
+        <v>1.7885888034340904</v>
+      </c>
+      <c r="J7" s="10">
+        <f t="shared" si="1"/>
+        <v>1.4492753623188408</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="1">
+        <f t="shared" ref="A8:A55" si="4">A7*1.18</f>
+        <v>4.177199999999999E-4</v>
+      </c>
+      <c r="B8" s="11">
+        <f t="shared" si="2"/>
+        <v>3.9734599363095171</v>
+      </c>
+      <c r="C8" s="11">
+        <f t="shared" si="0"/>
+        <v>7.7919925494657267</v>
+      </c>
+      <c r="D8" s="11">
+        <f t="shared" si="0"/>
+        <v>14.458676834838638</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+      <c r="G8" s="10">
+        <f>POWER((1-$H$4),F8)</f>
+        <v>0.99895036745712518</v>
+      </c>
+      <c r="H8" s="10">
+        <f t="shared" si="3"/>
+        <v>2.9905829604077674</v>
+      </c>
+      <c r="I8" s="10">
+        <f t="shared" si="1"/>
+        <v>2.3772148709053464</v>
+      </c>
+      <c r="J8" s="10">
+        <f t="shared" si="1"/>
+        <v>1.6547159404302263</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="1">
+        <f t="shared" si="4"/>
+        <v>4.929095999999998E-4</v>
+      </c>
+      <c r="B9" s="11">
+        <f t="shared" si="2"/>
+        <v>3.9687235829101333</v>
+      </c>
+      <c r="C9" s="11">
+        <f t="shared" si="0"/>
+        <v>7.7557569056202444</v>
+      </c>
+      <c r="D9" s="11">
+        <f t="shared" si="0"/>
+        <v>14.213132817023563</v>
+      </c>
+      <c r="F9">
+        <v>4</v>
+      </c>
+      <c r="G9" s="10">
+        <f>POWER((1-$H$4),F9)</f>
+        <v>0.99860073482851519</v>
+      </c>
+      <c r="H9" s="10">
+        <f t="shared" si="3"/>
+        <v>3.9777363681547704</v>
+      </c>
+      <c r="I9" s="10">
+        <f t="shared" si="1"/>
+        <v>2.7419256527407638</v>
+      </c>
+      <c r="J9" s="10">
+        <f t="shared" si="1"/>
+        <v>1.683785149014986</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="1">
+        <f t="shared" si="4"/>
+        <v>5.8163332799999968E-4</v>
+      </c>
+      <c r="B10" s="11">
+        <f t="shared" si="2"/>
+        <v>3.963150557710807</v>
+      </c>
+      <c r="C10" s="11">
+        <f t="shared" si="0"/>
+        <v>7.713454108373436</v>
+      </c>
+      <c r="D10" s="11">
+        <f t="shared" si="0"/>
+        <v>13.934243390154863</v>
+      </c>
+      <c r="F10">
+        <v>5</v>
+      </c>
+      <c r="G10" s="10">
+        <f>POWER((1-$H$4),F10)</f>
+        <v>0.9982512245713252</v>
+      </c>
+      <c r="H10" s="10">
+        <f t="shared" si="3"/>
+        <v>4.956659577611835</v>
+      </c>
+      <c r="I10" s="10">
+        <f t="shared" si="1"/>
+        <v>2.9302657613352339</v>
+      </c>
+      <c r="J10" s="10">
+        <f t="shared" si="1"/>
+        <v>1.6406621712523177</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="1">
+        <f t="shared" si="4"/>
+        <v>6.863273270399996E-4</v>
+      </c>
+      <c r="B11" s="11">
+        <f t="shared" si="2"/>
+        <v>3.9565963856503998</v>
+      </c>
+      <c r="C11" s="11">
+        <f t="shared" si="0"/>
+        <v>7.6641597427296579</v>
+      </c>
+      <c r="D11" s="11">
+        <f t="shared" si="0"/>
+        <v>13.619359411394994</v>
+      </c>
+      <c r="F11">
+        <v>6</v>
+      </c>
+      <c r="G11" s="10">
+        <f>POWER((1-$H$4),F11)</f>
+        <v>0.99790183664272536</v>
+      </c>
+      <c r="H11" s="10">
+        <f t="shared" si="3"/>
+        <v>5.9254051916986379</v>
+      </c>
+      <c r="I11" s="10">
+        <f t="shared" si="1"/>
+        <v>2.996751565615837</v>
+      </c>
+      <c r="J11" s="10">
+        <f t="shared" si="1"/>
+        <v>1.5742436939733233</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="1">
+        <f t="shared" si="4"/>
+        <v>8.0986624590719946E-4</v>
+      </c>
+      <c r="B12" s="11">
+        <f t="shared" si="2"/>
+        <v>3.948892925336458</v>
+      </c>
+      <c r="C12" s="11">
+        <f t="shared" si="0"/>
+        <v>7.6068421901071872</v>
+      </c>
+      <c r="D12" s="11">
+        <f t="shared" si="0"/>
+        <v>13.266215021163546</v>
+      </c>
+      <c r="F12">
+        <v>7</v>
+      </c>
+      <c r="G12" s="10">
+        <f>POWER((1-$H$4),F12)</f>
+        <v>0.99755257099990047</v>
+      </c>
+      <c r="H12" s="10">
+        <f t="shared" si="3"/>
+        <v>6.8820959121814251</v>
+      </c>
+      <c r="I12" s="10">
+        <f t="shared" si="1"/>
+        <v>2.9861951357431753</v>
+      </c>
+      <c r="J12" s="10">
+        <f t="shared" si="1"/>
+        <v>1.5047544759835492</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="1">
+        <f t="shared" si="4"/>
+        <v>9.5564217017049535E-4</v>
+      </c>
+      <c r="B13" s="11">
+        <f t="shared" si="2"/>
+        <v>3.9398449864966492</v>
+      </c>
+      <c r="C13" s="11">
+        <f t="shared" si="0"/>
+        <v>7.5403627063897423</v>
+      </c>
+      <c r="D13" s="11">
+        <f t="shared" si="0"/>
+        <v>12.873132291911777</v>
+      </c>
+      <c r="F13">
+        <v>8</v>
+      </c>
+      <c r="G13" s="10">
+        <f>POWER((1-$H$4),F13)</f>
+        <v>0.99720342760005054</v>
+      </c>
+      <c r="H13" s="10">
+        <f t="shared" si="3"/>
+        <v>7.8249359996168053</v>
+      </c>
+      <c r="I13" s="10">
+        <f t="shared" si="1"/>
+        <v>2.9303459072686611</v>
+      </c>
+      <c r="J13" s="10">
+        <f t="shared" si="1"/>
+        <v>1.4398168299584535</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="1">
+        <f t="shared" si="4"/>
+        <v>1.1276577608011844E-3</v>
+      </c>
+      <c r="B14" s="11">
+        <f t="shared" si="2"/>
+        <v>3.9292266577683952</v>
+      </c>
+      <c r="C14" s="11">
+        <f t="shared" si="0"/>
+        <v>7.4634809746527742</v>
+      </c>
+      <c r="D14" s="11">
+        <f t="shared" si="0"/>
+        <v>12.439245047431976</v>
+      </c>
+      <c r="F14">
+        <v>9</v>
+      </c>
+      <c r="G14" s="10">
+        <f>POWER((1-$H$4),F14)</f>
+        <v>0.99685440640039058</v>
+      </c>
+      <c r="H14" s="10">
+        <f t="shared" si="3"/>
+        <v>8.7522216095049998</v>
+      </c>
+      <c r="I14" s="10">
+        <f t="shared" si="1"/>
+        <v>2.849976774110984</v>
+      </c>
+      <c r="J14" s="10">
+        <f t="shared" si="1"/>
+        <v>1.3818059395088669</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="1">
+        <f t="shared" si="4"/>
+        <v>1.3306361577453975E-3</v>
+      </c>
+      <c r="B15" s="11">
+        <f t="shared" si="2"/>
+        <v>3.9167774026686337</v>
+      </c>
+      <c r="C15" s="11">
+        <f t="shared" si="0"/>
+        <v>7.3748681568595016</v>
+      </c>
+      <c r="D15" s="11">
+        <f t="shared" si="0"/>
+        <v>11.964724962144626</v>
+      </c>
+      <c r="F15">
+        <v>10</v>
+      </c>
+      <c r="G15" s="10">
+        <f>POWER((1-$H$4),F15)</f>
+        <v>0.99650550735815047</v>
+      </c>
+      <c r="H15" s="10">
+        <f>$F15/(((1-POWER((1-H$4),$F15))*($F15+1))+POWER((1-H$4),$F15))</f>
+        <v>9.6623498939269652</v>
+      </c>
+      <c r="I15" s="10">
+        <f t="shared" si="1"/>
+        <v>2.7580434170538628</v>
+      </c>
+      <c r="J15" s="10">
+        <f t="shared" si="1"/>
+        <v>1.330988026129716</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="1">
+        <f t="shared" si="4"/>
+        <v>1.570150666139569E-3</v>
+      </c>
+      <c r="B16" s="11">
+        <f t="shared" si="2"/>
+        <v>3.9021980261047458</v>
+      </c>
+      <c r="C16" s="11">
+        <f t="shared" si="0"/>
+        <v>7.273129742158126</v>
+      </c>
+      <c r="D16" s="11">
+        <f t="shared" si="0"/>
+        <v>11.450986226595836</v>
+      </c>
+      <c r="F16">
+        <v>11</v>
+      </c>
+      <c r="G16" s="10">
+        <f>POWER((1-$H$4),F16)</f>
+        <v>0.99615673043057518</v>
+      </c>
+      <c r="H16" s="10">
+        <f t="shared" si="3"/>
+        <v>10.55382678542073</v>
+      </c>
+      <c r="I16" s="10">
+        <f t="shared" si="1"/>
+        <v>2.6623523224490895</v>
+      </c>
+      <c r="J16" s="10">
+        <f t="shared" si="1"/>
+        <v>1.2868381635880028</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="1">
+        <f t="shared" si="4"/>
+        <v>1.8527777860446915E-3</v>
+      </c>
+      <c r="B17" s="11">
+        <f t="shared" si="2"/>
+        <v>3.8851466745588614</v>
+      </c>
+      <c r="C17" s="11">
+        <f t="shared" si="0"/>
+        <v>7.1568406053677123</v>
+      </c>
+      <c r="D17" s="11">
+        <f t="shared" si="0"/>
+        <v>10.900839884891164</v>
+      </c>
+      <c r="F17">
+        <v>12</v>
+      </c>
+      <c r="G17" s="10">
+        <f>POWER((1-$H$4),F17)</f>
+        <v>0.99580807557492457</v>
+      </c>
+      <c r="H17" s="10">
+        <f t="shared" si="3"/>
+        <v>11.42527340805149</v>
+      </c>
+      <c r="I17" s="10">
+        <f t="shared" si="1"/>
+        <v>2.5674536023198735</v>
+      </c>
+      <c r="J17" s="10">
+        <f t="shared" si="1"/>
+        <v>1.2485894110255731</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="1">
+        <f t="shared" si="4"/>
+        <v>2.186277787532736E-3</v>
+      </c>
+      <c r="B18" s="11">
+        <f t="shared" si="2"/>
+        <v>3.865235113528616</v>
+      </c>
+      <c r="C18" s="11">
+        <f t="shared" si="0"/>
+        <v>7.0245945212012506</v>
+      </c>
+      <c r="D18" s="11">
+        <f t="shared" si="0"/>
+        <v>10.318567405113988</v>
+      </c>
+      <c r="F18">
+        <v>13</v>
+      </c>
+      <c r="G18" s="10">
+        <f>POWER((1-$H$4),F18)</f>
+        <v>0.99545954274847326</v>
+      </c>
+      <c r="H18" s="10">
+        <f t="shared" si="3"/>
+        <v>12.275431088671708</v>
+      </c>
+      <c r="I18" s="10">
+        <f t="shared" si="1"/>
+        <v>2.4758849624331538</v>
+      </c>
+      <c r="J18" s="10">
+        <f t="shared" si="1"/>
+        <v>1.2154559900808217</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="1">
+        <f t="shared" si="4"/>
+        <v>2.5798077892886283E-3</v>
+      </c>
+      <c r="B19" s="11">
+        <f t="shared" si="2"/>
+        <v>3.8420256288902928</v>
+      </c>
+      <c r="C19" s="11">
+        <f t="shared" si="0"/>
+        <v>6.875069772481714</v>
+      </c>
+      <c r="D19" s="11">
+        <f t="shared" si="0"/>
+        <v>9.709886973641277</v>
+      </c>
+      <c r="F19">
+        <v>14</v>
+      </c>
+      <c r="G19" s="10">
+        <f>POWER((1-$H$4),F19)</f>
+        <v>0.99511113190851141</v>
+      </c>
+      <c r="H19" s="10">
+        <f t="shared" si="3"/>
+        <v>13.103164968436216</v>
+      </c>
+      <c r="I19" s="10">
+        <f t="shared" si="1"/>
+        <v>2.3889594108880869</v>
+      </c>
+      <c r="J19" s="10">
+        <f t="shared" si="1"/>
+        <v>1.1867173383541654</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="1">
+        <f t="shared" si="4"/>
+        <v>3.0441731913605813E-3</v>
+      </c>
+      <c r="B20" s="11">
+        <f t="shared" si="2"/>
+        <v>3.8150290260707793</v>
+      </c>
+      <c r="C20" s="11">
+        <f t="shared" si="0"/>
+        <v>6.7071112818789134</v>
+      </c>
+      <c r="D20" s="11">
+        <f t="shared" si="0"/>
+        <v>9.0817963477596741</v>
+      </c>
+      <c r="F20">
+        <v>15</v>
+      </c>
+      <c r="G20" s="10">
+        <f>POWER((1-$H$4),F20)</f>
+        <v>0.99476284301234352</v>
+      </c>
+      <c r="H20" s="10">
+        <f t="shared" si="3"/>
+        <v>13.907466240008169</v>
+      </c>
+      <c r="I20" s="10">
+        <f t="shared" si="1"/>
+        <v>2.3072549363008505</v>
+      </c>
+      <c r="J20" s="10">
+        <f t="shared" si="1"/>
+        <v>1.1617430559259629</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" s="1">
+        <f t="shared" si="4"/>
+        <v>3.5921243658054857E-3</v>
+      </c>
+      <c r="B21" s="11">
+        <f t="shared" si="2"/>
+        <v>3.7837043507873505</v>
+      </c>
+      <c r="C21" s="11">
+        <f t="shared" si="0"/>
+        <v>6.5198277611903572</v>
+      </c>
+      <c r="D21" s="11">
+        <f t="shared" si="0"/>
+        <v>8.4422921739859582</v>
+      </c>
+      <c r="F21">
+        <v>16</v>
+      </c>
+      <c r="G21" s="10">
+        <f>POWER((1-$H$4),F21)</f>
+        <v>0.99441467601728928</v>
+      </c>
+      <c r="H21" s="10">
+        <f t="shared" si="3"/>
+        <v>14.687453058957837</v>
+      </c>
+      <c r="I21" s="10">
+        <f t="shared" si="1"/>
+        <v>2.230916119506519</v>
+      </c>
+      <c r="J21" s="10">
+        <f t="shared" si="1"/>
+        <v>1.139993503780204</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="1">
+        <f t="shared" si="4"/>
+        <v>4.2387067516504728E-3</v>
+      </c>
+      <c r="B22" s="11">
+        <f t="shared" si="2"/>
+        <v>3.7474611209185928</v>
+      </c>
+      <c r="C22" s="11">
+        <f t="shared" si="2"/>
+        <v>6.312699689768686</v>
+      </c>
+      <c r="D22" s="11">
+        <f t="shared" si="2"/>
+        <v>7.7999848490006594</v>
+      </c>
+      <c r="F22">
+        <v>17</v>
+      </c>
+      <c r="G22" s="10">
+        <f>POWER((1-$H$4),F22)</f>
+        <v>0.99406663088068326</v>
+      </c>
+      <c r="H22" s="10">
+        <f t="shared" si="3"/>
+        <v>15.442370198134626</v>
+      </c>
+      <c r="I22" s="10">
+        <f t="shared" si="3"/>
+        <v>2.1598389434139067</v>
+      </c>
+      <c r="J22" s="10">
+        <f t="shared" si="3"/>
+        <v>1.121011244171761</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" s="1">
+        <f t="shared" si="4"/>
+        <v>5.0016739669475575E-3</v>
+      </c>
+      <c r="B23" s="11">
+        <f t="shared" si="2"/>
+        <v>3.7056650258807569</v>
+      </c>
+      <c r="C23" s="11">
+        <f t="shared" si="2"/>
+        <v>6.0856906746918371</v>
+      </c>
+      <c r="D23" s="11">
+        <f t="shared" si="2"/>
+        <v>7.1636460832409314</v>
+      </c>
+      <c r="F23">
+        <v>18</v>
+      </c>
+      <c r="G23" s="10">
+        <f>POWER((1-$H$4),F23)</f>
+        <v>0.99371870755987513</v>
+      </c>
+      <c r="H23" s="10">
+        <f t="shared" si="3"/>
+        <v>16.171587530946827</v>
+      </c>
+      <c r="I23" s="10">
+        <f t="shared" si="3"/>
+        <v>2.0937835246254726</v>
+      </c>
+      <c r="J23" s="10">
+        <f t="shared" si="3"/>
+        <v>1.1044098951442851</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="1">
+        <f t="shared" si="4"/>
+        <v>5.9019752809981174E-3</v>
+      </c>
+      <c r="B24" s="11">
+        <f t="shared" si="2"/>
+        <v>3.6576481910789269</v>
+      </c>
+      <c r="C24" s="11">
+        <f t="shared" si="2"/>
+        <v>5.8393513481504895</v>
+      </c>
+      <c r="D24" s="11">
+        <f t="shared" si="2"/>
+        <v>6.5417387565266809</v>
+      </c>
+      <c r="F24">
+        <v>19</v>
+      </c>
+      <c r="G24" s="10">
+        <f>POWER((1-$H$4),F24)</f>
+        <v>0.99337090601222922</v>
+      </c>
+      <c r="H24" s="10">
+        <f t="shared" si="3"/>
+        <v>16.874597443307803</v>
+      </c>
+      <c r="I24" s="10">
+        <f t="shared" si="3"/>
+        <v>2.0324424385364273</v>
+      </c>
+      <c r="J24" s="10">
+        <f t="shared" si="3"/>
+        <v>1.0898631308179154</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="1">
+        <f t="shared" si="4"/>
+        <v>6.9643308315777783E-3</v>
+      </c>
+      <c r="B25" s="11">
+        <f t="shared" si="2"/>
+        <v>3.6027251789257986</v>
+      </c>
+      <c r="C25" s="11">
+        <f t="shared" si="2"/>
+        <v>5.5749021554952449</v>
+      </c>
+      <c r="D25" s="11">
+        <f t="shared" si="2"/>
+        <v>5.9419820342839147</v>
+      </c>
+      <c r="F25">
+        <v>20</v>
+      </c>
+      <c r="G25" s="10">
+        <f>POWER((1-$H$4),F25)</f>
+        <v>0.99302322619512495</v>
+      </c>
+      <c r="H25" s="10">
+        <f t="shared" si="3"/>
+        <v>17.551011284433905</v>
+      </c>
+      <c r="I25" s="10">
+        <f t="shared" si="3"/>
+        <v>1.9754816763244711</v>
+      </c>
+      <c r="J25" s="10">
+        <f t="shared" si="3"/>
+        <v>1.0770948457344149</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="1">
+        <f t="shared" si="4"/>
+        <v>8.2179103812617775E-3</v>
+      </c>
+      <c r="B26" s="11">
+        <f t="shared" si="2"/>
+        <v>3.5402158460736493</v>
+      </c>
+      <c r="C26" s="11">
+        <f t="shared" si="2"/>
+        <v>5.2942801303429929</v>
+      </c>
+      <c r="D26" s="11">
+        <f t="shared" si="2"/>
+        <v>5.3709980882990429</v>
+      </c>
+      <c r="F26">
+        <v>21</v>
+      </c>
+      <c r="G26" s="10">
+        <f>POWER((1-$H$4),F26)</f>
+        <v>0.99267566806595664</v>
+      </c>
+      <c r="H26" s="10">
+        <f t="shared" si="3"/>
+        <v>18.200554973756475</v>
+      </c>
+      <c r="I26" s="10">
+        <f t="shared" si="3"/>
+        <v>1.9225647260267946</v>
+      </c>
+      <c r="J26" s="10">
+        <f t="shared" si="3"/>
+        <v>1.0658707500104958</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="1">
+        <f t="shared" si="4"/>
+        <v>9.6971342498888974E-3</v>
+      </c>
+      <c r="B27" s="11">
+        <f t="shared" si="2"/>
+        <v>3.4694759255641956</v>
+      </c>
+      <c r="C27" s="11">
+        <f t="shared" si="2"/>
+        <v>5.0001359873887257</v>
+      </c>
+      <c r="D27" s="11">
+        <f t="shared" si="2"/>
+        <v>4.8340719971445516</v>
+      </c>
+      <c r="F27">
+        <v>22</v>
+      </c>
+      <c r="G27" s="10">
+        <f>POWER((1-$H$4),F27)</f>
+        <v>0.99232823158213368</v>
+      </c>
+      <c r="H27" s="10">
+        <f t="shared" si="3"/>
+        <v>18.823063885094708</v>
+      </c>
+      <c r="I27" s="10">
+        <f t="shared" si="3"/>
+        <v>1.8733662553382437</v>
+      </c>
+      <c r="J27" s="10">
+        <f t="shared" si="3"/>
+        <v>1.0559913485486214</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="1">
+        <f t="shared" si="4"/>
+        <v>1.1442618414868898E-2</v>
+      </c>
+      <c r="B28" s="11">
+        <f t="shared" si="2"/>
+        <v>3.3899356733824164</v>
+      </c>
+      <c r="C28" s="11">
+        <f t="shared" si="2"/>
+        <v>4.6957721856226193</v>
+      </c>
+      <c r="D28" s="11">
+        <f t="shared" si="2"/>
+        <v>4.3350374435634222</v>
+      </c>
+      <c r="F28">
+        <v>23</v>
+      </c>
+      <c r="G28" s="10">
+        <f>POWER((1-$H$4),F28)</f>
+        <v>0.99198091670108002</v>
+      </c>
+      <c r="H28" s="10">
+        <f t="shared" si="3"/>
+        <v>19.418477130165666</v>
+      </c>
+      <c r="I28" s="10">
+        <f t="shared" si="3"/>
+        <v>1.8275794091858333</v>
+      </c>
+      <c r="J28" s="10">
+        <f t="shared" si="3"/>
+        <v>1.0472861426432427</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" s="1">
+        <f t="shared" si="4"/>
+        <v>1.3502289729545298E-2</v>
+      </c>
+      <c r="B29" s="11">
+        <f t="shared" si="2"/>
+        <v>3.3011460455667256</v>
+      </c>
+      <c r="C29" s="11">
+        <f t="shared" si="2"/>
+        <v>4.3850199000356715</v>
+      </c>
+      <c r="D29" s="11">
+        <f t="shared" si="2"/>
+        <v>3.8762822836677779</v>
+      </c>
+      <c r="F29">
+        <v>24</v>
+      </c>
+      <c r="G29" s="10">
+        <f>POWER((1-$H$4),F29)</f>
+        <v>0.99163372338023459</v>
+      </c>
+      <c r="H29" s="10">
+        <f t="shared" si="3"/>
+        <v>19.986831361791577</v>
+      </c>
+      <c r="I29" s="10">
+        <f t="shared" si="3"/>
+        <v>1.7849192165418508</v>
+      </c>
+      <c r="J29" s="10">
+        <f t="shared" si="3"/>
+        <v>1.0396088653228692</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="1">
+        <f t="shared" si="4"/>
+        <v>1.5932701880863452E-2</v>
+      </c>
+      <c r="B30" s="11">
+        <f t="shared" si="2"/>
+        <v>3.2028306332590479</v>
+      </c>
+      <c r="C30" s="11">
+        <f t="shared" si="2"/>
+        <v>4.0720620214518304</v>
+      </c>
+      <c r="D30" s="11">
+        <f t="shared" si="2"/>
+        <v>3.4588536976106439</v>
+      </c>
+      <c r="F30">
+        <v>25</v>
+      </c>
+      <c r="G30" s="10">
+        <f>POWER((1-$H$4),F30)</f>
+        <v>0.99128665157705165</v>
+      </c>
+      <c r="H30" s="10">
+        <f t="shared" si="3"/>
+        <v>20.52825421314931</v>
+      </c>
+      <c r="I30" s="10">
+        <f t="shared" si="3"/>
+        <v>1.7451236606298686</v>
+      </c>
+      <c r="J30" s="10">
+        <f t="shared" si="3"/>
+        <v>1.032833571396762</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" s="1">
+        <f t="shared" si="4"/>
+        <v>1.8800588219418872E-2</v>
+      </c>
+      <c r="B31" s="11">
+        <f t="shared" si="2"/>
+        <v>3.0949400425866331</v>
+      </c>
+      <c r="C31" s="11">
+        <f t="shared" si="2"/>
+        <v>3.7612184755962383</v>
+      </c>
+      <c r="D31" s="11">
+        <f t="shared" si="2"/>
+        <v>3.0826344305851845</v>
+      </c>
+      <c r="F31">
+        <v>26</v>
+      </c>
+      <c r="G31" s="10">
+        <f>POWER((1-$H$4),F31)</f>
+        <v>0.99093970124899966</v>
+      </c>
+      <c r="H31" s="10">
+        <f t="shared" si="3"/>
+        <v>21.04295748347344</v>
+      </c>
+      <c r="I31" s="10">
+        <f t="shared" si="3"/>
+        <v>1.7079533813867083</v>
+      </c>
+      <c r="J31" s="10">
+        <f t="shared" si="3"/>
+        <v>1.0268514258964598</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" s="1">
+        <f t="shared" si="4"/>
+        <v>2.2184694098914267E-2</v>
+      </c>
+      <c r="B32" s="11">
+        <f t="shared" si="2"/>
+        <v>2.9777037523799663</v>
+      </c>
+      <c r="C32" s="11">
+        <f t="shared" si="2"/>
+        <v>3.4567170594777799</v>
+      </c>
+      <c r="D32" s="11">
+        <f t="shared" si="2"/>
+        <v>2.7465596733245166</v>
+      </c>
+      <c r="F32">
+        <v>27</v>
+      </c>
+      <c r="G32" s="10">
+        <f>POWER((1-$H$4),F32)</f>
+        <v>0.99059287235356264</v>
+      </c>
+      <c r="H32" s="10">
+        <f t="shared" si="3"/>
+        <v>21.531230173159223</v>
+      </c>
+      <c r="I32" s="10">
+        <f t="shared" si="3"/>
+        <v>1.6731906129329981</v>
+      </c>
+      <c r="J32" s="10">
+        <f t="shared" si="3"/>
+        <v>1.0215680599444594</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="1">
+        <f t="shared" si="4"/>
+        <v>2.6177939036718834E-2</v>
+      </c>
+      <c r="B33" s="11">
+        <f t="shared" si="2"/>
+        <v>2.8516730474155874</v>
+      </c>
+      <c r="C33" s="11">
+        <f t="shared" si="2"/>
+        <v>3.1624757750948556</v>
+      </c>
+      <c r="D33" s="11">
+        <f t="shared" si="2"/>
+        <v>2.4488470791280683</v>
+      </c>
+      <c r="F33">
+        <v>28</v>
+      </c>
+      <c r="G33" s="10">
+        <f>POWER((1-$H$4),F33)</f>
+        <v>0.99024616484823891</v>
+      </c>
+      <c r="H33" s="10">
+        <f t="shared" si="3"/>
+        <v>21.993431462586511</v>
+      </c>
+      <c r="I33" s="10">
+        <f t="shared" si="3"/>
+        <v>1.6406377288546339</v>
+      </c>
+      <c r="J33" s="10">
+        <f t="shared" si="3"/>
+        <v>1.016901386707435</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" s="1">
+        <f t="shared" si="4"/>
+        <v>3.0889968063328221E-2</v>
+      </c>
+      <c r="B34" s="11">
+        <f t="shared" si="2"/>
+        <v>2.7177478564494333</v>
+      </c>
+      <c r="C34" s="11">
+        <f t="shared" si="2"/>
+        <v>2.8819205158596</v>
+      </c>
+      <c r="D34" s="11">
+        <f t="shared" si="2"/>
+        <v>2.1872182925771675</v>
+      </c>
+      <c r="F34">
+        <v>29</v>
+      </c>
+      <c r="G34" s="10">
+        <f>POWER((1-$H$4),F34)</f>
+        <v>0.98989957869054201</v>
+      </c>
+      <c r="H34" s="10">
+        <f t="shared" si="3"/>
+        <v>22.429983719572881</v>
+      </c>
+      <c r="I34" s="10">
+        <f t="shared" si="3"/>
+        <v>1.6101156232603391</v>
+      </c>
+      <c r="J34" s="10">
+        <f t="shared" si="3"/>
+        <v>1.0127797905005336</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" s="1">
+        <f t="shared" si="4"/>
+        <v>3.6450162314727301E-2</v>
+      </c>
+      <c r="B35" s="11">
+        <f t="shared" si="2"/>
+        <v>2.5771806930089132</v>
+      </c>
+      <c r="C35" s="11">
+        <f t="shared" si="2"/>
+        <v>2.6178555292347867</v>
+      </c>
+      <c r="D35" s="11">
+        <f t="shared" si="2"/>
+        <v>1.9590972386210093</v>
+      </c>
+      <c r="F35">
+        <v>30</v>
+      </c>
+      <c r="G35" s="10">
+        <f>POWER((1-$H$4),F35)</f>
+        <v>0.98955311383800038</v>
+      </c>
+      <c r="H35" s="10">
+        <f t="shared" si="3"/>
+        <v>22.841365610480814</v>
+      </c>
+      <c r="I35" s="10">
+        <f t="shared" si="3"/>
+        <v>1.5814620642585975</v>
+      </c>
+      <c r="J35" s="10">
+        <f t="shared" si="3"/>
+        <v>1.0091406190692729</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36" s="1">
+        <f t="shared" si="4"/>
+        <v>4.3011191531378209E-2</v>
+      </c>
+      <c r="B36" s="11">
+        <f t="shared" si="2"/>
+        <v>2.43155273537303</v>
+      </c>
+      <c r="C36" s="11">
+        <f t="shared" si="2"/>
+        <v>2.3723950860143317</v>
+      </c>
+      <c r="D36" s="11">
+        <f t="shared" si="2"/>
+        <v>1.761776814105108</v>
+      </c>
+      <c r="F36">
+        <v>31</v>
+      </c>
+      <c r="G36" s="10">
+        <f t="shared" ref="G36:G65" si="5">POWER((1-$H$4),F36)</f>
+        <v>0.98920677024815717</v>
+      </c>
+      <c r="H36" s="10">
+        <f t="shared" si="3"/>
+        <v>23.228105379957256</v>
+      </c>
+      <c r="I36" s="10">
+        <f t="shared" si="3"/>
+        <v>1.5545300989959976</v>
+      </c>
+      <c r="J36" s="10">
+        <f t="shared" si="3"/>
+        <v>1.005928922872132</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
+      <c r="A37" s="1">
+        <f t="shared" si="4"/>
+        <v>5.0753206007026284E-2</v>
+      </c>
+      <c r="B37" s="11">
+        <f t="shared" si="2"/>
+        <v>2.2827204022120346</v>
+      </c>
+      <c r="C37" s="11">
+        <f t="shared" si="2"/>
+        <v>2.1469554734197529</v>
+      </c>
+      <c r="D37" s="11">
+        <f t="shared" si="2"/>
+        <v>1.5925506504704781</v>
+      </c>
+      <c r="F37">
+        <v>32</v>
+      </c>
+      <c r="G37" s="10">
+        <f t="shared" si="5"/>
+        <v>0.98886054787857036</v>
+      </c>
+      <c r="H37" s="10">
+        <f t="shared" ref="H37:J52" si="6">$F37/(((1-POWER((1-H$4),$F37))*($F37+1))+POWER((1-H$4),$F37))</f>
+        <v>23.590774354322409</v>
+      </c>
+      <c r="I37" s="10">
+        <f t="shared" si="6"/>
+        <v>1.5291865533603282</v>
+      </c>
+      <c r="J37" s="10">
+        <f t="shared" si="6"/>
+        <v>1.0030963962772452</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" s="1">
+        <f t="shared" si="4"/>
+        <v>5.9888783088291014E-2</v>
+      </c>
+      <c r="B38" s="11">
+        <f t="shared" si="2"/>
+        <v>2.1327351461969037</v>
+      </c>
+      <c r="C38" s="11">
+        <f t="shared" si="2"/>
+        <v>1.9422987743082019</v>
+      </c>
+      <c r="D38" s="11">
+        <f t="shared" si="2"/>
+        <v>1.4488099069238174</v>
+      </c>
+      <c r="F38">
+        <v>33</v>
+      </c>
+      <c r="G38" s="10">
+        <f t="shared" si="5"/>
+        <v>0.98851444668681288</v>
+      </c>
+      <c r="H38" s="10">
+        <f t="shared" si="6"/>
+        <v>23.929980713965072</v>
+      </c>
+      <c r="I38" s="10">
+        <f t="shared" si="6"/>
+        <v>1.505310647071548</v>
+      </c>
+      <c r="J38" s="10">
+        <f t="shared" si="6"/>
+        <v>1.0006004844447771</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" s="1">
+        <f t="shared" si="4"/>
+        <v>7.0668764044183388E-2</v>
+      </c>
+      <c r="B39" s="11">
+        <f t="shared" ref="B39:D55" si="7">B$5/(((1-POWER((1-$A39),B$5))*(B$5+1))+(POWER((1-$A39),B$5)*1))</f>
+        <v>1.9837437345255258</v>
+      </c>
+      <c r="C39" s="11">
+        <f t="shared" si="7"/>
+        <v>1.7586150729858065</v>
+      </c>
+      <c r="D39" s="11">
+        <f t="shared" si="7"/>
+        <v>1.3281066007377373</v>
+      </c>
+      <c r="F39">
+        <v>34</v>
+      </c>
+      <c r="G39" s="10">
+        <f t="shared" si="5"/>
+        <v>0.98816846663047264</v>
+      </c>
+      <c r="H39" s="10">
+        <f t="shared" si="6"/>
+        <v>24.246363570914934</v>
+      </c>
+      <c r="I39" s="10">
+        <f t="shared" si="6"/>
+        <v>1.4827927312057174</v>
+      </c>
+      <c r="J39" s="10">
+        <f t="shared" si="6"/>
+        <v>0.99840362672084804</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="1">
+        <f t="shared" si="4"/>
+        <v>8.3389141572136394E-2</v>
+      </c>
+      <c r="B40" s="11">
+        <f t="shared" si="7"/>
+        <v>1.8378799255467377</v>
+      </c>
+      <c r="C40" s="11">
+        <f t="shared" si="7"/>
+        <v>1.5956279474108959</v>
+      </c>
+      <c r="D40" s="11">
+        <f t="shared" si="7"/>
+        <v>1.2281850088232034</v>
+      </c>
+      <c r="F40">
+        <v>35</v>
+      </c>
+      <c r="G40" s="10">
+        <f t="shared" si="5"/>
+        <v>0.98782260766715202</v>
+      </c>
+      <c r="H40" s="10">
+        <f t="shared" si="6"/>
+        <v>24.540587379181094</v>
+      </c>
+      <c r="I40" s="10">
+        <f t="shared" si="6"/>
+        <v>1.4615331470580128</v>
+      </c>
+      <c r="J40" s="10">
+        <f t="shared" si="6"/>
+        <v>0.99647261298240741</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41" s="1">
+        <f t="shared" si="4"/>
+        <v>9.8399187055120935E-2</v>
+      </c>
+      <c r="B41" s="11">
+        <f t="shared" si="7"/>
+        <v>1.6971602220179456</v>
+      </c>
+      <c r="C41" s="11">
+        <f t="shared" si="7"/>
+        <v>1.4527087854582896</v>
+      </c>
+      <c r="D41" s="11">
+        <f t="shared" si="7"/>
+        <v>1.1469816182050332</v>
+      </c>
+      <c r="F41">
+        <v>36</v>
+      </c>
+      <c r="G41" s="10">
+        <f t="shared" si="5"/>
+        <v>0.98747686975446847</v>
+      </c>
+      <c r="H41" s="10">
+        <f t="shared" si="6"/>
+        <v>24.813336697565678</v>
+      </c>
+      <c r="I41" s="10">
+        <f t="shared" si="6"/>
+        <v>1.4414412006242849</v>
+      </c>
+      <c r="J41" s="10">
+        <f t="shared" si="6"/>
+        <v>0.99477803384264052</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" s="1">
+        <f t="shared" si="4"/>
+        <v>0.11611104072504269</v>
+      </c>
+      <c r="B42" s="11">
+        <f t="shared" si="7"/>
+        <v>1.5633957936832548</v>
+      </c>
+      <c r="C42" s="11">
+        <f t="shared" si="7"/>
+        <v>1.3289875738055872</v>
+      </c>
+      <c r="D42" s="11">
+        <f t="shared" si="7"/>
+        <v>1.0825927929450734</v>
+      </c>
+      <c r="F42">
+        <v>37</v>
+      </c>
+      <c r="G42" s="10">
+        <f t="shared" si="5"/>
+        <v>0.98713125285005443</v>
+      </c>
+      <c r="H42" s="10">
+        <f t="shared" si="6"/>
+        <v>25.065311317537713</v>
+      </c>
+      <c r="I42" s="10">
+        <f t="shared" si="6"/>
+        <v>1.4224342445644216</v>
+      </c>
+      <c r="J42" s="10">
+        <f t="shared" si="6"/>
+        <v>0.99329380919228005</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43" s="1">
+        <f t="shared" si="4"/>
+        <v>0.13701102805555038</v>
+      </c>
+      <c r="B43" s="11">
+        <f t="shared" si="7"/>
+        <v>1.4381298795270481</v>
+      </c>
+      <c r="C43" s="11">
+        <f t="shared" si="7"/>
+        <v>1.2234502253828157</v>
+      </c>
+      <c r="D43" s="11">
+        <f t="shared" si="7"/>
+        <v>1.0332094230692521</v>
+      </c>
+      <c r="F43">
+        <v>38</v>
+      </c>
+      <c r="G43" s="10">
+        <f t="shared" si="5"/>
+        <v>0.98678575691155701</v>
+      </c>
+      <c r="H43" s="10">
+        <f t="shared" si="6"/>
+        <v>25.29722176242467</v>
+      </c>
+      <c r="I43" s="10">
+        <f t="shared" si="6"/>
+        <v>1.4044368584675841</v>
+      </c>
+      <c r="J43" s="10">
+        <f t="shared" si="6"/>
+        <v>0.99199678240333578</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="A44" s="1">
+        <f t="shared" si="4"/>
+        <v>0.16167301310554943</v>
+      </c>
+      <c r="B44" s="11">
+        <f t="shared" si="7"/>
+        <v>1.3226057447380477</v>
+      </c>
+      <c r="C44" s="11">
+        <f t="shared" si="7"/>
+        <v>1.1350142504724208</v>
+      </c>
+      <c r="D44" s="11">
+        <f t="shared" si="7"/>
+        <v>0.99702234613752172</v>
+      </c>
+      <c r="F44">
+        <v>39</v>
+      </c>
+      <c r="G44" s="10">
+        <f t="shared" si="5"/>
+        <v>0.98644038189663807</v>
+      </c>
+      <c r="H44" s="10">
+        <f t="shared" si="6"/>
+        <v>25.50978515864735</v>
+      </c>
+      <c r="I44" s="10">
+        <f t="shared" si="6"/>
+        <v>1.3873801180311174</v>
+      </c>
+      <c r="J44" s="10">
+        <f t="shared" si="6"/>
+        <v>0.99086636980796383</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="A45" s="1">
+        <f t="shared" si="4"/>
+        <v>0.19077415546454832</v>
+      </c>
+      <c r="B45" s="11">
+        <f t="shared" si="7"/>
+        <v>1.2177655865390256</v>
+      </c>
+      <c r="C45" s="11">
+        <f t="shared" si="7"/>
+        <v>1.0625749695482856</v>
+      </c>
+      <c r="D45" s="11">
+        <f t="shared" si="7"/>
+        <v>0.97211536434600643</v>
+      </c>
+      <c r="F45">
+        <v>40</v>
+      </c>
+      <c r="G45" s="10">
+        <f t="shared" si="5"/>
+        <v>0.98609512776297426</v>
+      </c>
+      <c r="H45" s="10">
+        <f t="shared" si="6"/>
+        <v>25.703721474975069</v>
+      </c>
+      <c r="I45" s="10">
+        <f t="shared" si="6"/>
+        <v>1.3712009440467443</v>
+      </c>
+      <c r="J45" s="10">
+        <f t="shared" si="6"/>
+        <v>0.98988425690426429</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="A46" s="1">
+        <f t="shared" si="4"/>
+        <v>0.225113503448167</v>
+      </c>
+      <c r="B46" s="11">
+        <f t="shared" si="7"/>
+        <v>1.1242765149213416</v>
+      </c>
+      <c r="C46" s="11">
+        <f t="shared" si="7"/>
+        <v>1.0050134524714667</v>
+      </c>
+      <c r="D46" s="11">
+        <f t="shared" si="7"/>
+        <v>0.95638592807687473</v>
+      </c>
+      <c r="F46">
+        <v>41</v>
+      </c>
+      <c r="G46" s="10">
+        <f t="shared" si="5"/>
+        <v>0.98574999446825728</v>
+      </c>
+      <c r="H46" s="10">
+        <f t="shared" si="6"/>
+        <v>25.87975012178325</v>
+      </c>
+      <c r="I46" s="10">
+        <f t="shared" si="6"/>
+        <v>1.355841522640048</v>
+      </c>
+      <c r="J46" s="10">
+        <f t="shared" si="6"/>
+        <v>0.98903413422516939</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="A47" s="1">
+        <f t="shared" si="4"/>
+        <v>0.26563393406883706</v>
+      </c>
+      <c r="B47" s="11">
+        <f t="shared" si="7"/>
+        <v>1.0425762051634602</v>
+      </c>
+      <c r="C47" s="11">
+        <f t="shared" si="7"/>
+        <v>0.96115626427768563</v>
+      </c>
+      <c r="D47" s="11">
+        <f t="shared" si="7"/>
+        <v>0.94755731504053164</v>
+      </c>
+      <c r="F47">
+        <v>42</v>
+      </c>
+      <c r="G47" s="10">
+        <f t="shared" si="5"/>
+        <v>0.98540498197019344</v>
+      </c>
+      <c r="H47" s="10">
+        <f t="shared" si="6"/>
+        <v>26.038586899008198</v>
+      </c>
+      <c r="I47" s="10">
+        <f t="shared" si="6"/>
+        <v>1.3412487888939819</v>
+      </c>
+      <c r="J47" s="10">
+        <f t="shared" si="6"/>
+        <v>0.98830146700897581</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
+      <c r="A48" s="1">
+        <f t="shared" si="4"/>
+        <v>0.31344804220122774</v>
+      </c>
+      <c r="B48" s="11">
+        <f t="shared" si="7"/>
+        <v>0.97292752071046018</v>
+      </c>
+      <c r="C48" s="11">
+        <f t="shared" si="7"/>
+        <v>0.92968026621566635</v>
+      </c>
+      <c r="D48" s="11">
+        <f t="shared" si="7"/>
+        <v>0.94333975568214079</v>
+      </c>
+      <c r="F48">
+        <v>43</v>
+      </c>
+      <c r="G48" s="10">
+        <f t="shared" si="5"/>
+        <v>0.98506009022650387</v>
+      </c>
+      <c r="H48" s="10">
+        <f t="shared" si="6"/>
+        <v>26.180941278866783</v>
+      </c>
+      <c r="I48" s="10">
+        <f t="shared" si="6"/>
+        <v>1.3273739667186311</v>
+      </c>
+      <c r="J48" s="10">
+        <f t="shared" si="6"/>
+        <v>0.98767329378760116</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
+      <c r="A49" s="1">
+        <f t="shared" si="4"/>
+        <v>0.36986868979744869</v>
+      </c>
+      <c r="B49" s="11">
+        <f t="shared" si="7"/>
+        <v>0.91546670689481624</v>
+      </c>
+      <c r="C49" s="11">
+        <f t="shared" si="7"/>
+        <v>0.90897273147402669</v>
+      </c>
+      <c r="D49" s="11">
+        <f t="shared" si="7"/>
+        <v>0.94172410622491065</v>
+      </c>
+      <c r="F49">
+        <v>44</v>
+      </c>
+      <c r="G49" s="10">
+        <f t="shared" si="5"/>
+        <v>0.98471531919492472</v>
+      </c>
+      <c r="H49" s="10">
+        <f t="shared" si="6"/>
+        <v>26.307514007376767</v>
+      </c>
+      <c r="I49" s="10">
+        <f t="shared" si="6"/>
+        <v>1.3141721585562061</v>
+      </c>
+      <c r="J49" s="10">
+        <f t="shared" si="6"/>
+        <v>0.9871380498063419</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
+      <c r="A50" s="1">
+        <f t="shared" si="4"/>
+        <v>0.43644505396098943</v>
+      </c>
+      <c r="B50" s="11">
+        <f t="shared" si="7"/>
+        <v>0.87022057778013118</v>
+      </c>
+      <c r="C50" s="11">
+        <f t="shared" si="7"/>
+        <v>0.89700093666640679</v>
+      </c>
+      <c r="D50" s="11">
+        <f t="shared" si="7"/>
+        <v>0.94126816960635495</v>
+      </c>
+      <c r="F50">
+        <v>45</v>
+      </c>
+      <c r="G50" s="10">
+        <f t="shared" si="5"/>
+        <v>0.98437066883320645</v>
+      </c>
+      <c r="H50" s="10">
+        <f t="shared" si="6"/>
+        <v>26.418995007221877</v>
+      </c>
+      <c r="I50" s="10">
+        <f t="shared" si="6"/>
+        <v>1.3016019792026199</v>
+      </c>
+      <c r="J50" s="10">
+        <f t="shared" si="6"/>
+        <v>0.98668541184233838</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
+      <c r="A51" s="1">
+        <f t="shared" si="4"/>
+        <v>0.51500516367396754</v>
+      </c>
+      <c r="B51" s="11">
+        <f t="shared" si="7"/>
+        <v>0.83705014589174243</v>
+      </c>
+      <c r="C51" s="11">
+        <f t="shared" si="7"/>
+        <v>0.8913142434806508</v>
+      </c>
+      <c r="D51" s="11">
+        <f t="shared" si="7"/>
+        <v>0.94118477176743243</v>
+      </c>
+      <c r="F51">
+        <v>46</v>
+      </c>
+      <c r="G51" s="10">
+        <f t="shared" si="5"/>
+        <v>0.98402613909911485</v>
+      </c>
+      <c r="H51" s="10">
+        <f t="shared" si="6"/>
+        <v>26.516061563491821</v>
+      </c>
+      <c r="I51" s="10">
+        <f t="shared" si="6"/>
+        <v>1.2896252286694134</v>
+      </c>
+      <c r="J51" s="10">
+        <f t="shared" si="6"/>
+        <v>0.98630616152625439</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
+      <c r="A52" s="1">
+        <f t="shared" si="4"/>
+        <v>0.60770609313528168</v>
+      </c>
+      <c r="B52" s="11">
+        <f t="shared" si="7"/>
+        <v>0.81545018461294405</v>
+      </c>
+      <c r="C52" s="11">
+        <f t="shared" si="7"/>
+        <v>0.88933229741909325</v>
+      </c>
+      <c r="D52" s="11">
+        <f t="shared" si="7"/>
+        <v>0.94117674928200123</v>
+      </c>
+      <c r="F52">
+        <v>47</v>
+      </c>
+      <c r="G52" s="10">
+        <f t="shared" si="5"/>
+        <v>0.98368172995043024</v>
+      </c>
+      <c r="H52" s="10">
+        <f t="shared" si="6"/>
+        <v>26.599376773222321</v>
+      </c>
+      <c r="I52" s="10">
+        <f t="shared" si="6"/>
+        <v>1.2782065995953029</v>
+      </c>
+      <c r="J52" s="10">
+        <f t="shared" si="6"/>
+        <v>0.98599206471519052</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
+      <c r="A53" s="1">
+        <f t="shared" si="4"/>
+        <v>0.71709318989963233</v>
+      </c>
+      <c r="B53" s="11">
+        <f t="shared" si="7"/>
+        <v>0.80412083198513451</v>
+      </c>
+      <c r="C53" s="11">
+        <f t="shared" si="7"/>
+        <v>0.88892131224835735</v>
+      </c>
+      <c r="D53" s="11">
+        <f t="shared" si="7"/>
+        <v>0.94117647207978083</v>
+      </c>
+      <c r="F53">
+        <v>48</v>
+      </c>
+      <c r="G53" s="10">
+        <f t="shared" si="5"/>
+        <v>0.98333744134494772</v>
+      </c>
+      <c r="H53" s="10">
+        <f t="shared" ref="H53:J65" si="8">$F53/(((1-POWER((1-H$4),$F53))*($F53+1))+POWER((1-H$4),$F53))</f>
+        <v>26.669588239419689</v>
+      </c>
+      <c r="I53" s="10">
+        <f t="shared" si="8"/>
+        <v>1.2673134152437897</v>
+      </c>
+      <c r="J53" s="10">
+        <f t="shared" si="8"/>
+        <v>0.98573576483236502</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
+      <c r="A54" s="1">
+        <f t="shared" si="4"/>
+        <v>0.84616996408156608</v>
+      </c>
+      <c r="B54" s="11">
+        <f t="shared" si="7"/>
+        <v>0.80035854125704298</v>
+      </c>
+      <c r="C54" s="11">
+        <f t="shared" si="7"/>
+        <v>0.88888913664490443</v>
+      </c>
+      <c r="D54" s="11">
+        <f t="shared" si="7"/>
+        <v>0.94117647058832243</v>
+      </c>
+      <c r="F54">
+        <v>49</v>
+      </c>
+      <c r="G54" s="10">
+        <f t="shared" si="5"/>
+        <v>0.98299327324047703</v>
+      </c>
+      <c r="H54" s="10">
+        <f t="shared" si="8"/>
+        <v>26.727326990307457</v>
+      </c>
+      <c r="I54" s="10">
+        <f t="shared" si="8"/>
+        <v>1.2569153945938067</v>
+      </c>
+      <c r="J54" s="10">
+        <f t="shared" si="8"/>
+        <v>0.98553068839482716</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
+      <c r="A55" s="1">
+        <f t="shared" si="4"/>
+        <v>0.99848055761624788</v>
+      </c>
+      <c r="B55" s="11">
+        <f t="shared" si="7"/>
+        <v>0.80000000000341132</v>
+      </c>
+      <c r="C55" s="11">
+        <f t="shared" si="7"/>
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="D55" s="11">
+        <f t="shared" si="7"/>
+        <v>0.94117647058823528</v>
+      </c>
+      <c r="F55">
+        <v>50</v>
+      </c>
+      <c r="G55" s="10">
+        <f t="shared" si="5"/>
+        <v>0.98264922559484291</v>
+      </c>
+      <c r="H55" s="10">
+        <f t="shared" si="8"/>
+        <v>26.773206604838915</v>
+      </c>
+      <c r="I55" s="10">
+        <f t="shared" si="8"/>
+        <v>1.2469844414477198</v>
+      </c>
+      <c r="J55" s="10">
+        <f t="shared" si="8"/>
+        <v>0.98537096120576029</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10">
+      <c r="F56">
+        <v>51</v>
+      </c>
+      <c r="G56" s="10">
+        <f t="shared" si="5"/>
+        <v>0.98230529836588476</v>
+      </c>
+      <c r="H56" s="10">
+        <f t="shared" si="8"/>
+        <v>26.807822526025202</v>
+      </c>
+      <c r="I56" s="10">
+        <f t="shared" si="8"/>
+        <v>1.237494454849583</v>
+      </c>
+      <c r="J56" s="10">
+        <f t="shared" si="8"/>
+        <v>0.98525133390195796</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10">
+      <c r="F57">
+        <v>52</v>
+      </c>
+      <c r="G57" s="10">
+        <f t="shared" si="5"/>
+        <v>0.98196149151145673</v>
+      </c>
+      <c r="H57" s="10">
+        <f t="shared" si="8"/>
+        <v>26.831751544297081</v>
+      </c>
+      <c r="I57" s="10">
+        <f t="shared" si="8"/>
+        <v>1.2284211584309919</v>
+      </c>
+      <c r="J57" s="10">
+        <f t="shared" si="8"/>
+        <v>0.9851671157271511</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10">
+      <c r="F58">
+        <v>53</v>
+      </c>
+      <c r="G58" s="10">
+        <f t="shared" si="5"/>
+        <v>0.98161780498942774</v>
+      </c>
+      <c r="H58" s="10">
+        <f t="shared" si="8"/>
+        <v>26.845551433906198</v>
+      </c>
+      <c r="I58" s="10">
+        <f t="shared" si="8"/>
+        <v>1.2197419465868915</v>
+      </c>
+      <c r="J58" s="10">
+        <f t="shared" si="8"/>
+        <v>0.98511411555399708</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10">
+      <c r="F59">
+        <v>54</v>
+      </c>
+      <c r="G59" s="10">
+        <f t="shared" si="5"/>
+        <v>0.9812742387576816</v>
+      </c>
+      <c r="H59" s="10">
+        <f t="shared" si="8"/>
+        <v>26.849760726250356</v>
+      </c>
+      <c r="I59" s="10">
+        <f t="shared" si="8"/>
+        <v>1.2114357456336868</v>
+      </c>
+      <c r="J59" s="10">
+        <f t="shared" si="8"/>
+        <v>0.98508858930653032</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10">
+      <c r="F60">
+        <v>55</v>
+      </c>
+      <c r="G60" s="10">
+        <f t="shared" si="5"/>
+        <v>0.98093079277411643</v>
+      </c>
+      <c r="H60" s="10">
+        <f t="shared" si="8"/>
+        <v>26.844898604945445</v>
+      </c>
+      <c r="I60" s="10">
+        <f t="shared" si="8"/>
+        <v>1.2034828883210924</v>
+      </c>
+      <c r="J60" s="10">
+        <f t="shared" si="8"/>
+        <v>0.98508719304463321</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10">
+      <c r="F61">
+        <v>56</v>
+      </c>
+      <c r="G61" s="10">
+        <f t="shared" si="5"/>
+        <v>0.98058746699664545</v>
+      </c>
+      <c r="H61" s="10">
+        <f t="shared" si="8"/>
+        <v>26.8314649084435</v>
+      </c>
+      <c r="I61" s="10">
+        <f t="shared" si="8"/>
+        <v>1.1958650002610993</v>
+      </c>
+      <c r="J61" s="10">
+        <f t="shared" si="8"/>
+        <v>0.98510694106584906</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10">
+      <c r="F62">
+        <v>57</v>
+      </c>
+      <c r="G62" s="10">
+        <f t="shared" si="5"/>
+        <v>0.98024426138319676</v>
+      </c>
+      <c r="H62" s="10">
+        <f t="shared" si="8"/>
+        <v>26.809940226984175</v>
+      </c>
+      <c r="I62" s="10">
+        <f t="shared" si="8"/>
+        <v>1.1885648970055627</v>
+      </c>
+      <c r="J62" s="10">
+        <f t="shared" si="8"/>
+        <v>0.98514516846019895</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10">
+      <c r="F63">
+        <v>58</v>
+      </c>
+      <c r="G63" s="10">
+        <f t="shared" si="5"/>
+        <v>0.97990117589171266</v>
+      </c>
+      <c r="H63" s="10">
+        <f t="shared" si="8"/>
+        <v>26.780786081658462</v>
+      </c>
+      <c r="I63" s="10">
+        <f t="shared" si="8"/>
+        <v>1.1815664906512133</v>
+      </c>
+      <c r="J63" s="10">
+        <f t="shared" si="8"/>
+        <v>0.98519949762277725</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10">
+      <c r="F64">
+        <v>59</v>
+      </c>
+      <c r="G64" s="10">
+        <f t="shared" si="5"/>
+        <v>0.97955821048015068</v>
+      </c>
+      <c r="H64" s="10">
+        <f t="shared" si="8"/>
+        <v>26.744445174339333</v>
+      </c>
+      <c r="I64" s="10">
+        <f t="shared" si="8"/>
+        <v>1.1748547049800309</v>
+      </c>
+      <c r="J64" s="10">
+        <f t="shared" si="8"/>
+        <v>0.98526780828852678</v>
+      </c>
+    </row>
+    <row r="65" spans="6:10">
+      <c r="F65">
+        <v>60</v>
+      </c>
+      <c r="G65" s="10">
+        <f t="shared" si="5"/>
+        <v>0.97921536510648266</v>
+      </c>
+      <c r="H65" s="10">
+        <f t="shared" si="8"/>
+        <v>26.701341698178535</v>
+      </c>
+      <c r="I65" s="10">
+        <f t="shared" si="8"/>
+        <v>1.1684153982561554</v>
+      </c>
+      <c r="J65" s="10">
+        <f t="shared" si="8"/>
+        <v>0.98534821070521916</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>